<commit_message>
updated generation to include multiple properties in one workbook
</commit_message>
<xml_diff>
--- a/break_even_template.xlsx
+++ b/break_even_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brandonhightower/PycharmProjects/AION-make-ready/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04DC6B64-A512-7540-8288-BCBC3E0343CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D4042BC-BA49-FC41-9802-06CA8C637BB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19240" yWindow="-20940" windowWidth="38100" windowHeight="20800" xr2:uid="{0749BF83-3DEB-384E-B1FF-6FE42BFA2EA4}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="34560" windowHeight="22340" xr2:uid="{0749BF83-3DEB-384E-B1FF-6FE42BFA2EA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="2" r:id="rId1"/>
@@ -116,9 +116,6 @@
     <t>/ # of workdays in period</t>
   </si>
   <si>
-    <t>=AVG daily work orders opened</t>
-  </si>
-  <si>
     <t>Total pending work orders</t>
   </si>
   <si>
@@ -132,6 +129,9 @@
   </si>
   <si>
     <t>Required daily work order output *In addition to Break even ( 0.0 per-workday)*</t>
+  </si>
+  <si>
+    <t>AVG daily work orders opened</t>
   </si>
 </sst>
 </file>
@@ -914,12 +914,34 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="21" xfId="6" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="6" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="28" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="29" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="37" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="38" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="33" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="32" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="34" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -968,28 +990,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="33" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="6" borderId="32" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="6" borderId="34" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="37" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="38" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="40% - Accent1" xfId="4" builtinId="31"/>
@@ -1334,7 +1334,7 @@
   <dimension ref="A2:P65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1364,13 +1364,13 @@
       <c r="A3" s="3"/>
       <c r="B3" s="2"/>
       <c r="C3" s="3"/>
-      <c r="D3" s="65" t="s">
+      <c r="D3" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
+      <c r="E3" s="73"/>
+      <c r="F3" s="73"/>
+      <c r="G3" s="73"/>
+      <c r="H3" s="73"/>
     </row>
     <row r="4" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -1383,11 +1383,11 @@
       <c r="C4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="66"/>
-      <c r="E4" s="67"/>
-      <c r="F4" s="67"/>
-      <c r="G4" s="67"/>
-      <c r="H4" s="68"/>
+      <c r="D4" s="74"/>
+      <c r="E4" s="75"/>
+      <c r="F4" s="75"/>
+      <c r="G4" s="75"/>
+      <c r="H4" s="76"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
@@ -1436,10 +1436,10 @@
       <c r="B8" s="6"/>
       <c r="C8" s="3"/>
       <c r="L8" s="12"/>
-      <c r="M8" s="69"/>
-      <c r="N8" s="69"/>
-      <c r="O8" s="69"/>
-      <c r="P8" s="70"/>
+      <c r="M8" s="77"/>
+      <c r="N8" s="77"/>
+      <c r="O8" s="77"/>
+      <c r="P8" s="78"/>
     </row>
     <row r="9" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
@@ -1482,12 +1482,12 @@
       <c r="H11" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="L11" s="71" t="s">
+      <c r="L11" s="79" t="s">
         <v>17</v>
       </c>
-      <c r="M11" s="72"/>
-      <c r="N11" s="72"/>
-      <c r="O11" s="72"/>
+      <c r="M11" s="80"/>
+      <c r="N11" s="80"/>
+      <c r="O11" s="80"/>
       <c r="P11" s="20" t="s">
         <v>18</v>
       </c>
@@ -1504,15 +1504,15 @@
         <v>21.666666666666668</v>
       </c>
       <c r="I12" s="23"/>
-      <c r="L12" s="73" t="s">
-        <v>31</v>
-      </c>
-      <c r="M12" s="75" t="s">
+      <c r="L12" s="81" t="s">
+        <v>30</v>
+      </c>
+      <c r="M12" s="83" t="s">
         <v>19</v>
       </c>
-      <c r="N12" s="76"/>
-      <c r="O12" s="76"/>
-      <c r="P12" s="79" t="s">
+      <c r="N12" s="84"/>
+      <c r="O12" s="84"/>
+      <c r="P12" s="87" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1536,11 +1536,11 @@
       </c>
       <c r="H13" s="28"/>
       <c r="I13" s="23"/>
-      <c r="L13" s="74"/>
-      <c r="M13" s="77"/>
-      <c r="N13" s="78"/>
-      <c r="O13" s="78"/>
-      <c r="P13" s="80"/>
+      <c r="L13" s="82"/>
+      <c r="M13" s="85"/>
+      <c r="N13" s="86"/>
+      <c r="O13" s="86"/>
+      <c r="P13" s="88"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="29" t="s">
@@ -1562,12 +1562,12 @@
       <c r="L14" s="32">
         <v>1</v>
       </c>
-      <c r="M14" s="63">
+      <c r="M14" s="64">
         <f>$B$15/G12*22</f>
         <v>0</v>
       </c>
-      <c r="N14" s="64"/>
-      <c r="O14" s="64"/>
+      <c r="N14" s="65"/>
+      <c r="O14" s="65"/>
       <c r="P14" s="33">
         <f t="shared" ref="P14:P65" si="0">L14+$B$24</f>
         <v>1</v>
@@ -1586,7 +1586,7 @@
       <c r="F15" s="26">
         <v>4</v>
       </c>
-      <c r="G15" s="88">
+      <c r="G15" s="63">
         <v>86.666666666666671</v>
       </c>
       <c r="H15" s="28"/>
@@ -1594,12 +1594,12 @@
       <c r="L15" s="32">
         <v>2</v>
       </c>
-      <c r="M15" s="63">
+      <c r="M15" s="64">
         <f t="shared" ref="M15:M65" si="1">$B$15/G13*22</f>
         <v>0</v>
       </c>
-      <c r="N15" s="64"/>
-      <c r="O15" s="64"/>
+      <c r="N15" s="65"/>
+      <c r="O15" s="65"/>
       <c r="P15" s="33">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -1613,7 +1613,7 @@
       <c r="F16" s="26">
         <v>5</v>
       </c>
-      <c r="G16" s="88">
+      <c r="G16" s="63">
         <v>108.33333333333334</v>
       </c>
       <c r="H16" s="28"/>
@@ -1621,12 +1621,12 @@
       <c r="L16" s="32">
         <v>3</v>
       </c>
-      <c r="M16" s="63">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N16" s="64"/>
-      <c r="O16" s="64"/>
+      <c r="M16" s="64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N16" s="65"/>
+      <c r="O16" s="65"/>
       <c r="P16" s="33">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -1645,7 +1645,7 @@
       <c r="F17" s="26">
         <v>6</v>
       </c>
-      <c r="G17" s="88">
+      <c r="G17" s="63">
         <v>130</v>
       </c>
       <c r="H17" s="28"/>
@@ -1653,12 +1653,12 @@
       <c r="L17" s="32">
         <v>4</v>
       </c>
-      <c r="M17" s="63">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N17" s="64"/>
-      <c r="O17" s="64"/>
+      <c r="M17" s="64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N17" s="65"/>
+      <c r="O17" s="65"/>
       <c r="P17" s="33">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1676,19 +1676,19 @@
       <c r="F18" s="26">
         <v>7</v>
       </c>
-      <c r="G18" s="88">
+      <c r="G18" s="63">
         <v>151.66666666666669</v>
       </c>
       <c r="H18" s="28"/>
       <c r="L18" s="40">
         <v>5</v>
       </c>
-      <c r="M18" s="63">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N18" s="64"/>
-      <c r="O18" s="64"/>
+      <c r="M18" s="64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N18" s="65"/>
+      <c r="O18" s="65"/>
       <c r="P18" s="33">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1696,7 +1696,7 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" s="34" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B19" s="41">
         <f>B17/B18</f>
@@ -1715,12 +1715,12 @@
       <c r="L19" s="32">
         <v>6</v>
       </c>
-      <c r="M19" s="63">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N19" s="64"/>
-      <c r="O19" s="64"/>
+      <c r="M19" s="64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N19" s="65"/>
+      <c r="O19" s="65"/>
       <c r="P19" s="33">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1742,12 +1742,12 @@
       <c r="L20" s="32">
         <v>7</v>
       </c>
-      <c r="M20" s="63">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N20" s="64"/>
-      <c r="O20" s="64"/>
+      <c r="M20" s="64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N20" s="65"/>
+      <c r="O20" s="65"/>
       <c r="P20" s="33">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1755,7 +1755,7 @@
     </row>
     <row r="21" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="43" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B21" s="36">
         <f>O9</f>
@@ -1772,12 +1772,12 @@
       <c r="L21" s="32">
         <v>8</v>
       </c>
-      <c r="M21" s="63">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N21" s="64"/>
-      <c r="O21" s="64"/>
+      <c r="M21" s="64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N21" s="65"/>
+      <c r="O21" s="65"/>
       <c r="P21" s="33">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1785,7 +1785,7 @@
     </row>
     <row r="22" spans="1:16" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B22" s="42">
         <v>278</v>
@@ -1801,12 +1801,12 @@
       <c r="L22" s="32">
         <v>9</v>
       </c>
-      <c r="M22" s="63">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N22" s="64"/>
-      <c r="O22" s="64"/>
+      <c r="M22" s="64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N22" s="65"/>
+      <c r="O22" s="65"/>
       <c r="P22" s="33">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1814,7 +1814,7 @@
     </row>
     <row r="23" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B23" s="46">
         <f>B21/B22</f>
@@ -1831,26 +1831,26 @@
       <c r="L23" s="32">
         <v>10</v>
       </c>
-      <c r="M23" s="63">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N23" s="64"/>
-      <c r="O23" s="64"/>
+      <c r="M23" s="64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N23" s="65"/>
+      <c r="O23" s="65"/>
       <c r="P23" s="33">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A24" s="81" t="s">
-        <v>30</v>
-      </c>
-      <c r="B24" s="83">
+      <c r="A24" s="68" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="70">
         <f>B17/B6</f>
         <v>0</v>
       </c>
-      <c r="C24" s="85"/>
+      <c r="C24" s="72"/>
       <c r="F24" s="44">
         <v>13</v>
       </c>
@@ -1861,21 +1861,21 @@
       <c r="L24" s="32">
         <v>11</v>
       </c>
-      <c r="M24" s="63">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N24" s="64"/>
-      <c r="O24" s="64"/>
+      <c r="M24" s="64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N24" s="65"/>
+      <c r="O24" s="65"/>
       <c r="P24" s="33">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="82"/>
-      <c r="B25" s="84"/>
-      <c r="C25" s="85"/>
+      <c r="A25" s="69"/>
+      <c r="B25" s="71"/>
+      <c r="C25" s="72"/>
       <c r="E25" s="25"/>
       <c r="F25">
         <v>14</v>
@@ -1887,12 +1887,12 @@
       <c r="L25" s="47">
         <v>12</v>
       </c>
-      <c r="M25" s="63">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N25" s="64"/>
-      <c r="O25" s="64"/>
+      <c r="M25" s="64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N25" s="65"/>
+      <c r="O25" s="65"/>
       <c r="P25" s="33">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1910,12 +1910,12 @@
       <c r="L26" s="47">
         <v>13</v>
       </c>
-      <c r="M26" s="63">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N26" s="64"/>
-      <c r="O26" s="64"/>
+      <c r="M26" s="64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N26" s="65"/>
+      <c r="O26" s="65"/>
       <c r="P26" s="33">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1933,12 +1933,12 @@
       <c r="L27" s="47">
         <v>14</v>
       </c>
-      <c r="M27" s="63">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N27" s="64"/>
-      <c r="O27" s="64"/>
+      <c r="M27" s="64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N27" s="65"/>
+      <c r="O27" s="65"/>
       <c r="P27" s="33">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1956,12 +1956,12 @@
       <c r="L28" s="47">
         <v>15</v>
       </c>
-      <c r="M28" s="63">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N28" s="64"/>
-      <c r="O28" s="64"/>
+      <c r="M28" s="64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N28" s="65"/>
+      <c r="O28" s="65"/>
       <c r="P28" s="33">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1979,12 +1979,12 @@
       <c r="L29" s="47">
         <v>16</v>
       </c>
-      <c r="M29" s="63">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N29" s="64"/>
-      <c r="O29" s="64"/>
+      <c r="M29" s="64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N29" s="65"/>
+      <c r="O29" s="65"/>
       <c r="P29" s="33">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -2001,12 +2001,12 @@
       <c r="L30" s="47">
         <v>17</v>
       </c>
-      <c r="M30" s="63">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N30" s="64"/>
-      <c r="O30" s="64"/>
+      <c r="M30" s="64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N30" s="65"/>
+      <c r="O30" s="65"/>
       <c r="P30" s="33">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -2023,12 +2023,12 @@
       <c r="L31" s="47">
         <v>18</v>
       </c>
-      <c r="M31" s="63">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N31" s="64"/>
-      <c r="O31" s="64"/>
+      <c r="M31" s="64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N31" s="65"/>
+      <c r="O31" s="65"/>
       <c r="P31" s="33">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -2046,12 +2046,12 @@
       <c r="L32" s="47">
         <v>19</v>
       </c>
-      <c r="M32" s="63">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N32" s="64"/>
-      <c r="O32" s="64"/>
+      <c r="M32" s="64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N32" s="65"/>
+      <c r="O32" s="65"/>
       <c r="P32" s="33">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -2068,12 +2068,12 @@
       <c r="L33" s="47">
         <v>20</v>
       </c>
-      <c r="M33" s="63">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N33" s="64"/>
-      <c r="O33" s="64"/>
+      <c r="M33" s="64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N33" s="65"/>
+      <c r="O33" s="65"/>
       <c r="P33" s="33">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -2090,12 +2090,12 @@
       <c r="L34" s="47">
         <v>21</v>
       </c>
-      <c r="M34" s="63">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N34" s="64"/>
-      <c r="O34" s="64"/>
+      <c r="M34" s="64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N34" s="65"/>
+      <c r="O34" s="65"/>
       <c r="P34" s="33">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -2112,12 +2112,12 @@
       <c r="L35" s="47">
         <v>22</v>
       </c>
-      <c r="M35" s="63">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N35" s="64"/>
-      <c r="O35" s="64"/>
+      <c r="M35" s="64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N35" s="65"/>
+      <c r="O35" s="65"/>
       <c r="P35" s="33">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -2134,12 +2134,12 @@
       <c r="L36" s="47">
         <v>23</v>
       </c>
-      <c r="M36" s="63">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N36" s="64"/>
-      <c r="O36" s="64"/>
+      <c r="M36" s="64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N36" s="65"/>
+      <c r="O36" s="65"/>
       <c r="P36" s="33">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -2157,12 +2157,12 @@
       <c r="L37" s="47">
         <v>24</v>
       </c>
-      <c r="M37" s="63">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N37" s="64"/>
-      <c r="O37" s="64"/>
+      <c r="M37" s="64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N37" s="65"/>
+      <c r="O37" s="65"/>
       <c r="P37" s="33">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -2181,12 +2181,12 @@
       <c r="L38" s="32">
         <v>25</v>
       </c>
-      <c r="M38" s="63">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N38" s="64"/>
-      <c r="O38" s="64"/>
+      <c r="M38" s="64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N38" s="65"/>
+      <c r="O38" s="65"/>
       <c r="P38" s="33">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -2203,12 +2203,12 @@
       <c r="L39" s="32">
         <v>26</v>
       </c>
-      <c r="M39" s="63">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N39" s="64"/>
-      <c r="O39" s="64"/>
+      <c r="M39" s="64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N39" s="65"/>
+      <c r="O39" s="65"/>
       <c r="P39" s="33">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -2225,12 +2225,12 @@
       <c r="L40" s="47">
         <v>27</v>
       </c>
-      <c r="M40" s="63">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N40" s="64"/>
-      <c r="O40" s="64"/>
+      <c r="M40" s="64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N40" s="65"/>
+      <c r="O40" s="65"/>
       <c r="P40" s="33">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -2247,12 +2247,12 @@
       <c r="L41" s="47">
         <v>28</v>
       </c>
-      <c r="M41" s="63">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N41" s="64"/>
-      <c r="O41" s="64"/>
+      <c r="M41" s="64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N41" s="65"/>
+      <c r="O41" s="65"/>
       <c r="P41" s="33">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -2269,12 +2269,12 @@
       <c r="L42" s="32">
         <v>29</v>
       </c>
-      <c r="M42" s="63">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N42" s="64"/>
-      <c r="O42" s="64"/>
+      <c r="M42" s="64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N42" s="65"/>
+      <c r="O42" s="65"/>
       <c r="P42" s="33">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -2291,12 +2291,12 @@
       <c r="L43" s="32">
         <v>30</v>
       </c>
-      <c r="M43" s="63">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N43" s="64"/>
-      <c r="O43" s="64"/>
+      <c r="M43" s="64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N43" s="65"/>
+      <c r="O43" s="65"/>
       <c r="P43" s="33">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -2313,12 +2313,12 @@
       <c r="L44" s="47">
         <v>31</v>
       </c>
-      <c r="M44" s="63">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N44" s="64"/>
-      <c r="O44" s="64"/>
+      <c r="M44" s="64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N44" s="65"/>
+      <c r="O44" s="65"/>
       <c r="P44" s="33">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -2335,12 +2335,12 @@
       <c r="L45" s="32">
         <v>32</v>
       </c>
-      <c r="M45" s="63">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N45" s="64"/>
-      <c r="O45" s="64"/>
+      <c r="M45" s="64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N45" s="65"/>
+      <c r="O45" s="65"/>
       <c r="P45" s="33">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -2357,12 +2357,12 @@
       <c r="L46" s="32">
         <v>33</v>
       </c>
-      <c r="M46" s="63">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N46" s="64"/>
-      <c r="O46" s="64"/>
+      <c r="M46" s="64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N46" s="65"/>
+      <c r="O46" s="65"/>
       <c r="P46" s="33">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -2379,12 +2379,12 @@
       <c r="L47" s="32">
         <v>34</v>
       </c>
-      <c r="M47" s="63">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N47" s="64"/>
-      <c r="O47" s="64"/>
+      <c r="M47" s="64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N47" s="65"/>
+      <c r="O47" s="65"/>
       <c r="P47" s="33">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -2401,12 +2401,12 @@
       <c r="L48" s="47">
         <v>35</v>
       </c>
-      <c r="M48" s="63">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N48" s="64"/>
-      <c r="O48" s="64"/>
+      <c r="M48" s="64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N48" s="65"/>
+      <c r="O48" s="65"/>
       <c r="P48" s="33">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -2423,12 +2423,12 @@
       <c r="L49" s="47">
         <v>36</v>
       </c>
-      <c r="M49" s="63">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N49" s="64"/>
-      <c r="O49" s="64"/>
+      <c r="M49" s="64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N49" s="65"/>
+      <c r="O49" s="65"/>
       <c r="P49" s="33">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -2445,12 +2445,12 @@
       <c r="L50" s="32">
         <v>37</v>
       </c>
-      <c r="M50" s="63">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N50" s="64"/>
-      <c r="O50" s="64"/>
+      <c r="M50" s="64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N50" s="65"/>
+      <c r="O50" s="65"/>
       <c r="P50" s="33">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -2467,12 +2467,12 @@
       <c r="L51" s="32">
         <v>38</v>
       </c>
-      <c r="M51" s="63">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N51" s="64"/>
-      <c r="O51" s="64"/>
+      <c r="M51" s="64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N51" s="65"/>
+      <c r="O51" s="65"/>
       <c r="P51" s="33">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -2489,12 +2489,12 @@
       <c r="L52" s="47">
         <v>39</v>
       </c>
-      <c r="M52" s="63">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N52" s="64"/>
-      <c r="O52" s="64"/>
+      <c r="M52" s="64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N52" s="65"/>
+      <c r="O52" s="65"/>
       <c r="P52" s="33">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -2511,12 +2511,12 @@
       <c r="L53" s="47">
         <v>40</v>
       </c>
-      <c r="M53" s="63">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N53" s="64"/>
-      <c r="O53" s="64"/>
+      <c r="M53" s="64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N53" s="65"/>
+      <c r="O53" s="65"/>
       <c r="P53" s="33">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -2533,12 +2533,12 @@
       <c r="L54" s="32">
         <v>41</v>
       </c>
-      <c r="M54" s="63">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N54" s="64"/>
-      <c r="O54" s="64"/>
+      <c r="M54" s="64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N54" s="65"/>
+      <c r="O54" s="65"/>
       <c r="P54" s="33">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -2555,12 +2555,12 @@
       <c r="L55" s="32">
         <v>42</v>
       </c>
-      <c r="M55" s="63">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N55" s="64"/>
-      <c r="O55" s="64"/>
+      <c r="M55" s="64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N55" s="65"/>
+      <c r="O55" s="65"/>
       <c r="P55" s="33">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -2577,12 +2577,12 @@
       <c r="L56" s="47">
         <v>43</v>
       </c>
-      <c r="M56" s="63">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N56" s="64"/>
-      <c r="O56" s="64"/>
+      <c r="M56" s="64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N56" s="65"/>
+      <c r="O56" s="65"/>
       <c r="P56" s="33">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -2599,12 +2599,12 @@
       <c r="L57" s="47">
         <v>44</v>
       </c>
-      <c r="M57" s="63">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N57" s="64"/>
-      <c r="O57" s="64"/>
+      <c r="M57" s="64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N57" s="65"/>
+      <c r="O57" s="65"/>
       <c r="P57" s="33">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -2621,12 +2621,12 @@
       <c r="L58" s="32">
         <v>45</v>
       </c>
-      <c r="M58" s="63">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N58" s="64"/>
-      <c r="O58" s="64"/>
+      <c r="M58" s="64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N58" s="65"/>
+      <c r="O58" s="65"/>
       <c r="P58" s="33">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -2643,12 +2643,12 @@
       <c r="L59" s="32">
         <v>46</v>
       </c>
-      <c r="M59" s="63">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N59" s="64"/>
-      <c r="O59" s="64"/>
+      <c r="M59" s="64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N59" s="65"/>
+      <c r="O59" s="65"/>
       <c r="P59" s="33">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -2665,12 +2665,12 @@
       <c r="L60" s="47">
         <v>47</v>
       </c>
-      <c r="M60" s="63">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N60" s="64"/>
-      <c r="O60" s="64"/>
+      <c r="M60" s="64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N60" s="65"/>
+      <c r="O60" s="65"/>
       <c r="P60" s="33">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -2687,12 +2687,12 @@
       <c r="L61" s="47">
         <v>48</v>
       </c>
-      <c r="M61" s="63">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N61" s="64"/>
-      <c r="O61" s="64"/>
+      <c r="M61" s="64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N61" s="65"/>
+      <c r="O61" s="65"/>
       <c r="P61" s="33">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -2709,12 +2709,12 @@
       <c r="L62" s="32">
         <v>49</v>
       </c>
-      <c r="M62" s="63">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N62" s="64"/>
-      <c r="O62" s="64"/>
+      <c r="M62" s="64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N62" s="65"/>
+      <c r="O62" s="65"/>
       <c r="P62" s="33">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -2731,12 +2731,12 @@
       <c r="L63" s="32">
         <v>50</v>
       </c>
-      <c r="M63" s="63">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N63" s="64"/>
-      <c r="O63" s="64"/>
+      <c r="M63" s="64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N63" s="65"/>
+      <c r="O63" s="65"/>
       <c r="P63" s="33">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -2746,12 +2746,12 @@
       <c r="L64" s="32">
         <v>51</v>
       </c>
-      <c r="M64" s="63">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N64" s="64"/>
-      <c r="O64" s="64"/>
+      <c r="M64" s="64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N64" s="65"/>
+      <c r="O64" s="65"/>
       <c r="P64" s="33">
         <f t="shared" si="0"/>
         <v>51</v>
@@ -2761,12 +2761,12 @@
       <c r="L65" s="54">
         <v>52</v>
       </c>
-      <c r="M65" s="86">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N65" s="87"/>
-      <c r="O65" s="87"/>
+      <c r="M65" s="66">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N65" s="67"/>
+      <c r="O65" s="67"/>
       <c r="P65" s="55">
         <f t="shared" si="0"/>
         <v>52</v>
@@ -2774,55 +2774,6 @@
     </row>
   </sheetData>
   <mergeCells count="62">
-    <mergeCell ref="M62:O62"/>
-    <mergeCell ref="M63:O63"/>
-    <mergeCell ref="M64:O64"/>
-    <mergeCell ref="M65:O65"/>
-    <mergeCell ref="M56:O56"/>
-    <mergeCell ref="M57:O57"/>
-    <mergeCell ref="M58:O58"/>
-    <mergeCell ref="M59:O59"/>
-    <mergeCell ref="M60:O60"/>
-    <mergeCell ref="M61:O61"/>
-    <mergeCell ref="M55:O55"/>
-    <mergeCell ref="M44:O44"/>
-    <mergeCell ref="M45:O45"/>
-    <mergeCell ref="M46:O46"/>
-    <mergeCell ref="M47:O47"/>
-    <mergeCell ref="M48:O48"/>
-    <mergeCell ref="M49:O49"/>
-    <mergeCell ref="M50:O50"/>
-    <mergeCell ref="M51:O51"/>
-    <mergeCell ref="M52:O52"/>
-    <mergeCell ref="M53:O53"/>
-    <mergeCell ref="M54:O54"/>
-    <mergeCell ref="M43:O43"/>
-    <mergeCell ref="M32:O32"/>
-    <mergeCell ref="M33:O33"/>
-    <mergeCell ref="M34:O34"/>
-    <mergeCell ref="M35:O35"/>
-    <mergeCell ref="M36:O36"/>
-    <mergeCell ref="M37:O37"/>
-    <mergeCell ref="M38:O38"/>
-    <mergeCell ref="M39:O39"/>
-    <mergeCell ref="M40:O40"/>
-    <mergeCell ref="M41:O41"/>
-    <mergeCell ref="M42:O42"/>
-    <mergeCell ref="M31:O31"/>
-    <mergeCell ref="M20:O20"/>
-    <mergeCell ref="M21:O21"/>
-    <mergeCell ref="M22:O22"/>
-    <mergeCell ref="M23:O23"/>
-    <mergeCell ref="M26:O26"/>
-    <mergeCell ref="M27:O27"/>
-    <mergeCell ref="M28:O28"/>
-    <mergeCell ref="M29:O29"/>
-    <mergeCell ref="M30:O30"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="M24:O24"/>
-    <mergeCell ref="M25:O25"/>
     <mergeCell ref="M19:O19"/>
     <mergeCell ref="D3:H3"/>
     <mergeCell ref="D4:H4"/>
@@ -2836,6 +2787,55 @@
     <mergeCell ref="M16:O16"/>
     <mergeCell ref="M17:O17"/>
     <mergeCell ref="M18:O18"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="M24:O24"/>
+    <mergeCell ref="M25:O25"/>
+    <mergeCell ref="M31:O31"/>
+    <mergeCell ref="M20:O20"/>
+    <mergeCell ref="M21:O21"/>
+    <mergeCell ref="M22:O22"/>
+    <mergeCell ref="M23:O23"/>
+    <mergeCell ref="M26:O26"/>
+    <mergeCell ref="M27:O27"/>
+    <mergeCell ref="M28:O28"/>
+    <mergeCell ref="M29:O29"/>
+    <mergeCell ref="M30:O30"/>
+    <mergeCell ref="M43:O43"/>
+    <mergeCell ref="M32:O32"/>
+    <mergeCell ref="M33:O33"/>
+    <mergeCell ref="M34:O34"/>
+    <mergeCell ref="M35:O35"/>
+    <mergeCell ref="M36:O36"/>
+    <mergeCell ref="M37:O37"/>
+    <mergeCell ref="M38:O38"/>
+    <mergeCell ref="M39:O39"/>
+    <mergeCell ref="M40:O40"/>
+    <mergeCell ref="M41:O41"/>
+    <mergeCell ref="M42:O42"/>
+    <mergeCell ref="M55:O55"/>
+    <mergeCell ref="M44:O44"/>
+    <mergeCell ref="M45:O45"/>
+    <mergeCell ref="M46:O46"/>
+    <mergeCell ref="M47:O47"/>
+    <mergeCell ref="M48:O48"/>
+    <mergeCell ref="M49:O49"/>
+    <mergeCell ref="M50:O50"/>
+    <mergeCell ref="M51:O51"/>
+    <mergeCell ref="M52:O52"/>
+    <mergeCell ref="M53:O53"/>
+    <mergeCell ref="M54:O54"/>
+    <mergeCell ref="M62:O62"/>
+    <mergeCell ref="M63:O63"/>
+    <mergeCell ref="M64:O64"/>
+    <mergeCell ref="M65:O65"/>
+    <mergeCell ref="M56:O56"/>
+    <mergeCell ref="M57:O57"/>
+    <mergeCell ref="M58:O58"/>
+    <mergeCell ref="M59:O59"/>
+    <mergeCell ref="M60:O60"/>
+    <mergeCell ref="M61:O61"/>
   </mergeCells>
   <conditionalFormatting sqref="M14:M65">
     <cfRule type="dataBar" priority="16">

</xml_diff>

<commit_message>
format fix for template
</commit_message>
<xml_diff>
--- a/break_even_template.xlsx
+++ b/break_even_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brandonhightower/PycharmProjects/AION-make-ready/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D4042BC-BA49-FC41-9802-06CA8C637BB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A594F893-0153-8E44-8A4B-3A7FAD0E3D3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="34560" windowHeight="22340" xr2:uid="{0749BF83-3DEB-384E-B1FF-6FE42BFA2EA4}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20380" xr2:uid="{0749BF83-3DEB-384E-B1FF-6FE42BFA2EA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="2" r:id="rId1"/>
@@ -107,9 +107,6 @@
     <t xml:space="preserve"> *Work days in a month (AVG)</t>
   </si>
   <si>
-    <t>=Work orders completed per-month (AVG)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Work order inflow </t>
   </si>
   <si>
@@ -132,6 +129,9 @@
   </si>
   <si>
     <t>AVG daily work orders opened</t>
+  </si>
+  <si>
+    <t>Work orders completed per-month (AVG)</t>
   </si>
 </sst>
 </file>
@@ -921,74 +921,74 @@
     <xf numFmtId="164" fontId="8" fillId="0" borderId="29" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="9" fillId="0" borderId="12" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="9" fillId="0" borderId="13" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="18" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="19" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="33" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="32" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="34" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="37" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="38" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="33" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="6" borderId="32" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="6" borderId="34" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="9" fillId="0" borderId="12" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="9" fillId="0" borderId="13" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="18" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="19" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1334,7 +1334,7 @@
   <dimension ref="A2:P65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1364,13 +1364,13 @@
       <c r="A3" s="3"/>
       <c r="B3" s="2"/>
       <c r="C3" s="3"/>
-      <c r="D3" s="73" t="s">
+      <c r="D3" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="73"/>
-      <c r="F3" s="73"/>
-      <c r="G3" s="73"/>
-      <c r="H3" s="73"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="66"/>
     </row>
     <row r="4" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -1383,11 +1383,11 @@
       <c r="C4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="74"/>
-      <c r="E4" s="75"/>
-      <c r="F4" s="75"/>
-      <c r="G4" s="75"/>
-      <c r="H4" s="76"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="68"/>
+      <c r="F4" s="68"/>
+      <c r="G4" s="68"/>
+      <c r="H4" s="69"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
@@ -1436,10 +1436,10 @@
       <c r="B8" s="6"/>
       <c r="C8" s="3"/>
       <c r="L8" s="12"/>
-      <c r="M8" s="77"/>
-      <c r="N8" s="77"/>
-      <c r="O8" s="77"/>
-      <c r="P8" s="78"/>
+      <c r="M8" s="70"/>
+      <c r="N8" s="70"/>
+      <c r="O8" s="70"/>
+      <c r="P8" s="71"/>
     </row>
     <row r="9" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
@@ -1482,12 +1482,12 @@
       <c r="H11" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="L11" s="79" t="s">
+      <c r="L11" s="72" t="s">
         <v>17</v>
       </c>
-      <c r="M11" s="80"/>
-      <c r="N11" s="80"/>
-      <c r="O11" s="80"/>
+      <c r="M11" s="73"/>
+      <c r="N11" s="73"/>
+      <c r="O11" s="73"/>
       <c r="P11" s="20" t="s">
         <v>18</v>
       </c>
@@ -1504,15 +1504,15 @@
         <v>21.666666666666668</v>
       </c>
       <c r="I12" s="23"/>
-      <c r="L12" s="81" t="s">
-        <v>30</v>
-      </c>
-      <c r="M12" s="83" t="s">
+      <c r="L12" s="74" t="s">
+        <v>29</v>
+      </c>
+      <c r="M12" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="N12" s="84"/>
-      <c r="O12" s="84"/>
-      <c r="P12" s="87" t="s">
+      <c r="N12" s="77"/>
+      <c r="O12" s="77"/>
+      <c r="P12" s="80" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1536,11 +1536,11 @@
       </c>
       <c r="H13" s="28"/>
       <c r="I13" s="23"/>
-      <c r="L13" s="82"/>
-      <c r="M13" s="85"/>
-      <c r="N13" s="86"/>
-      <c r="O13" s="86"/>
-      <c r="P13" s="88"/>
+      <c r="L13" s="75"/>
+      <c r="M13" s="78"/>
+      <c r="N13" s="79"/>
+      <c r="O13" s="79"/>
+      <c r="P13" s="81"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="29" t="s">
@@ -1575,7 +1575,7 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="34" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B15" s="24">
         <f>B13*B14</f>
@@ -1634,7 +1634,7 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B17" s="36">
         <f>M9</f>
@@ -1666,7 +1666,7 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" s="37" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B18" s="36">
         <f>B6</f>
@@ -1696,7 +1696,7 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" s="34" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B19" s="41">
         <f>B17/B18</f>
@@ -1755,7 +1755,7 @@
     </row>
     <row r="21" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="43" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B21" s="36">
         <f>O9</f>
@@ -1785,7 +1785,7 @@
     </row>
     <row r="22" spans="1:16" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B22" s="42">
         <v>278</v>
@@ -1814,7 +1814,7 @@
     </row>
     <row r="23" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B23" s="46">
         <f>B21/B22</f>
@@ -1843,14 +1843,14 @@
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A24" s="68" t="s">
-        <v>29</v>
-      </c>
-      <c r="B24" s="70">
+      <c r="A24" s="82" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="84">
         <f>B17/B6</f>
         <v>0</v>
       </c>
-      <c r="C24" s="72"/>
+      <c r="C24" s="86"/>
       <c r="F24" s="44">
         <v>13</v>
       </c>
@@ -1873,9 +1873,9 @@
       </c>
     </row>
     <row r="25" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="69"/>
-      <c r="B25" s="71"/>
-      <c r="C25" s="72"/>
+      <c r="A25" s="83"/>
+      <c r="B25" s="85"/>
+      <c r="C25" s="86"/>
       <c r="E25" s="25"/>
       <c r="F25">
         <v>14</v>
@@ -2761,12 +2761,12 @@
       <c r="L65" s="54">
         <v>52</v>
       </c>
-      <c r="M65" s="66">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N65" s="67"/>
-      <c r="O65" s="67"/>
+      <c r="M65" s="87">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N65" s="88"/>
+      <c r="O65" s="88"/>
       <c r="P65" s="55">
         <f t="shared" si="0"/>
         <v>52</v>
@@ -2774,6 +2774,55 @@
     </row>
   </sheetData>
   <mergeCells count="62">
+    <mergeCell ref="M62:O62"/>
+    <mergeCell ref="M63:O63"/>
+    <mergeCell ref="M64:O64"/>
+    <mergeCell ref="M65:O65"/>
+    <mergeCell ref="M56:O56"/>
+    <mergeCell ref="M57:O57"/>
+    <mergeCell ref="M58:O58"/>
+    <mergeCell ref="M59:O59"/>
+    <mergeCell ref="M60:O60"/>
+    <mergeCell ref="M61:O61"/>
+    <mergeCell ref="M55:O55"/>
+    <mergeCell ref="M44:O44"/>
+    <mergeCell ref="M45:O45"/>
+    <mergeCell ref="M46:O46"/>
+    <mergeCell ref="M47:O47"/>
+    <mergeCell ref="M48:O48"/>
+    <mergeCell ref="M49:O49"/>
+    <mergeCell ref="M50:O50"/>
+    <mergeCell ref="M51:O51"/>
+    <mergeCell ref="M52:O52"/>
+    <mergeCell ref="M53:O53"/>
+    <mergeCell ref="M54:O54"/>
+    <mergeCell ref="M43:O43"/>
+    <mergeCell ref="M32:O32"/>
+    <mergeCell ref="M33:O33"/>
+    <mergeCell ref="M34:O34"/>
+    <mergeCell ref="M35:O35"/>
+    <mergeCell ref="M36:O36"/>
+    <mergeCell ref="M37:O37"/>
+    <mergeCell ref="M38:O38"/>
+    <mergeCell ref="M39:O39"/>
+    <mergeCell ref="M40:O40"/>
+    <mergeCell ref="M41:O41"/>
+    <mergeCell ref="M42:O42"/>
+    <mergeCell ref="M31:O31"/>
+    <mergeCell ref="M20:O20"/>
+    <mergeCell ref="M21:O21"/>
+    <mergeCell ref="M22:O22"/>
+    <mergeCell ref="M23:O23"/>
+    <mergeCell ref="M26:O26"/>
+    <mergeCell ref="M27:O27"/>
+    <mergeCell ref="M28:O28"/>
+    <mergeCell ref="M29:O29"/>
+    <mergeCell ref="M30:O30"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="M24:O24"/>
+    <mergeCell ref="M25:O25"/>
     <mergeCell ref="M19:O19"/>
     <mergeCell ref="D3:H3"/>
     <mergeCell ref="D4:H4"/>
@@ -2787,55 +2836,6 @@
     <mergeCell ref="M16:O16"/>
     <mergeCell ref="M17:O17"/>
     <mergeCell ref="M18:O18"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="M24:O24"/>
-    <mergeCell ref="M25:O25"/>
-    <mergeCell ref="M31:O31"/>
-    <mergeCell ref="M20:O20"/>
-    <mergeCell ref="M21:O21"/>
-    <mergeCell ref="M22:O22"/>
-    <mergeCell ref="M23:O23"/>
-    <mergeCell ref="M26:O26"/>
-    <mergeCell ref="M27:O27"/>
-    <mergeCell ref="M28:O28"/>
-    <mergeCell ref="M29:O29"/>
-    <mergeCell ref="M30:O30"/>
-    <mergeCell ref="M43:O43"/>
-    <mergeCell ref="M32:O32"/>
-    <mergeCell ref="M33:O33"/>
-    <mergeCell ref="M34:O34"/>
-    <mergeCell ref="M35:O35"/>
-    <mergeCell ref="M36:O36"/>
-    <mergeCell ref="M37:O37"/>
-    <mergeCell ref="M38:O38"/>
-    <mergeCell ref="M39:O39"/>
-    <mergeCell ref="M40:O40"/>
-    <mergeCell ref="M41:O41"/>
-    <mergeCell ref="M42:O42"/>
-    <mergeCell ref="M55:O55"/>
-    <mergeCell ref="M44:O44"/>
-    <mergeCell ref="M45:O45"/>
-    <mergeCell ref="M46:O46"/>
-    <mergeCell ref="M47:O47"/>
-    <mergeCell ref="M48:O48"/>
-    <mergeCell ref="M49:O49"/>
-    <mergeCell ref="M50:O50"/>
-    <mergeCell ref="M51:O51"/>
-    <mergeCell ref="M52:O52"/>
-    <mergeCell ref="M53:O53"/>
-    <mergeCell ref="M54:O54"/>
-    <mergeCell ref="M62:O62"/>
-    <mergeCell ref="M63:O63"/>
-    <mergeCell ref="M64:O64"/>
-    <mergeCell ref="M65:O65"/>
-    <mergeCell ref="M56:O56"/>
-    <mergeCell ref="M57:O57"/>
-    <mergeCell ref="M58:O58"/>
-    <mergeCell ref="M59:O59"/>
-    <mergeCell ref="M60:O60"/>
-    <mergeCell ref="M61:O61"/>
   </mergeCells>
   <conditionalFormatting sqref="M14:M65">
     <cfRule type="dataBar" priority="16">

</xml_diff>